<commit_message>
Update before i change the upload to get default password
</commit_message>
<xml_diff>
--- a/Cyber_Kitchen/DataUploadTemplates/StaffNamesample.xlsx
+++ b/Cyber_Kitchen/DataUploadTemplates/StaffNamesample.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>CBY001</t>
   </si>
@@ -39,13 +39,19 @@
   </si>
   <si>
     <t>Tobi Adeogun</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>michael.aruebo@cyberspace.net.ng</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -53,6 +59,12 @@
     <font>
       <sz val="10"/>
       <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -120,11 +132,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -135,8 +148,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Sheet1" xfId="1"/>
   </cellStyles>
@@ -440,36 +455,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="42" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -477,12 +498,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>